<commit_message>
More additional topics for arrays
</commit_message>
<xml_diff>
--- a/src/main/frontend/Basic Frontend - Homestudy links.xlsx
+++ b/src/main/frontend/Basic Frontend - Homestudy links.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="145">
   <si>
     <t xml:space="preserve">Базовый HTML + CSS</t>
   </si>
@@ -390,9 +390,6 @@
     <t xml:space="preserve">https://learn.javascript.ru/while-for</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">https://youtu.be/ITr-SzUIDpQ</t>
   </si>
   <si>
@@ -463,6 +460,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://developer.mozilla.org/ru/docs/Web/JavaScript/Guide/Indexed_collections</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://learn.javascript.ru/array
+http://learn.javascript.ru/array-methods
+http://learn.javascript.ru/array-iteration
+http://learn.javascript.ru/arguments-pseudoarray</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">﻿</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/3OjuRfR8RNg</t>
@@ -592,7 +613,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -628,6 +649,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lohit Devanagari"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -731,13 +758,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="75.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="93.92"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="2" width="11.52"/>
@@ -1076,76 +1103,74 @@
       <c r="C22" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="71.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="6" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>109</v>
@@ -1280,9 +1305,7 @@
       <c r="C34" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>89</v>
-      </c>
+      <c r="D34" s="7"/>
       <c r="E34" s="6" t="s">
         <v>139</v>
       </c>
@@ -1297,9 +1320,7 @@
       <c r="C35" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>89</v>
-      </c>
+      <c r="D35" s="7"/>
       <c r="E35" s="6" t="s">
         <v>144</v>
       </c>
@@ -1317,21 +1338,22 @@
     <hyperlink ref="E24" r:id="rId9" display="https://youtu.be/J1aIrZFnGig"/>
     <hyperlink ref="E25" r:id="rId10" display="https://youtu.be/213r4EOHfF0"/>
     <hyperlink ref="C26" r:id="rId11" display="https://developer.mozilla.org/ru/docs/Web/JavaScript/Guide/Indexed_collections"/>
-    <hyperlink ref="E26" r:id="rId12" display="https://youtu.be/3OjuRfR8RNg"/>
-    <hyperlink ref="E27" r:id="rId13" display="https://youtu.be/SbPtW-hiWZI"/>
-    <hyperlink ref="E28" r:id="rId14" display="https://youtu.be/KEsA5wAg5Xc"/>
-    <hyperlink ref="D29" r:id="rId15" display="https://learn.javascript.ru/multi-insert"/>
-    <hyperlink ref="E29" r:id="rId16" display="https://www.youtube.com/watch?v=1FpuKVmotNc"/>
-    <hyperlink ref="E30" r:id="rId17" display="https://www.youtube.com/watch?v=8cV4ZvHXQL4"/>
-    <hyperlink ref="E31" r:id="rId18" display="https://www.youtube.com/watch?v=8cV4ZvHXQL4"/>
-    <hyperlink ref="D32" r:id="rId19" display="http://htmlbook.ru/html5/storage"/>
-    <hyperlink ref="E32" r:id="rId20" display="https://www.youtube.com/watch?v=puxkpNbCh0w"/>
-    <hyperlink ref="C33" r:id="rId21" display="https://api.jquery.com/"/>
-    <hyperlink ref="E33" r:id="rId22" display="https://www.youtube.com/watch?v=B4jWRrz3FUM&amp;list=PLVfMKQXDAhGXQcouhIblV910Rv7lRscH3"/>
-    <hyperlink ref="C34" r:id="rId23" display="https://api.jquery.com/"/>
-    <hyperlink ref="E34" r:id="rId24" display="https://www.youtube.com/watch?v=B4jWRrz3FUM&amp;list=PLVfMKQXDAhGXQcouhIblV910Rv7lRscH3"/>
-    <hyperlink ref="C35" r:id="rId25" display="https://webhamster.ru/mytetrashare/index/mtb0/4115"/>
-    <hyperlink ref="E35" r:id="rId26" display="https://www.youtube.com/watch?v=rD-V7bXoq88"/>
+    <hyperlink ref="D26" r:id="rId12" display="http://learn.javascript.ru/arguments-pseudoarray"/>
+    <hyperlink ref="E26" r:id="rId13" display="https://youtu.be/3OjuRfR8RNg"/>
+    <hyperlink ref="E27" r:id="rId14" display="https://youtu.be/SbPtW-hiWZI"/>
+    <hyperlink ref="E28" r:id="rId15" display="https://youtu.be/KEsA5wAg5Xc"/>
+    <hyperlink ref="D29" r:id="rId16" display="https://learn.javascript.ru/multi-insert"/>
+    <hyperlink ref="E29" r:id="rId17" display="https://www.youtube.com/watch?v=1FpuKVmotNc"/>
+    <hyperlink ref="E30" r:id="rId18" display="https://www.youtube.com/watch?v=8cV4ZvHXQL4"/>
+    <hyperlink ref="E31" r:id="rId19" display="https://www.youtube.com/watch?v=8cV4ZvHXQL4"/>
+    <hyperlink ref="D32" r:id="rId20" display="http://htmlbook.ru/html5/storage"/>
+    <hyperlink ref="E32" r:id="rId21" display="https://www.youtube.com/watch?v=puxkpNbCh0w"/>
+    <hyperlink ref="C33" r:id="rId22" display="https://api.jquery.com/"/>
+    <hyperlink ref="E33" r:id="rId23" display="https://www.youtube.com/watch?v=B4jWRrz3FUM&amp;list=PLVfMKQXDAhGXQcouhIblV910Rv7lRscH3"/>
+    <hyperlink ref="C34" r:id="rId24" display="https://api.jquery.com/"/>
+    <hyperlink ref="E34" r:id="rId25" display="https://www.youtube.com/watch?v=B4jWRrz3FUM&amp;list=PLVfMKQXDAhGXQcouhIblV910Rv7lRscH3"/>
+    <hyperlink ref="C35" r:id="rId26" display="https://webhamster.ru/mytetrashare/index/mtb0/4115"/>
+    <hyperlink ref="E35" r:id="rId27" display="https://www.youtube.com/watch?v=rD-V7bXoq88"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>